<commit_message>
implement site change requests
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2572" uniqueCount="1491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="1494">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -1932,18 +1932,18 @@
     <t xml:space="preserve">Masculino</t>
   </si>
   <si>
+    <t xml:space="preserve">Me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feminino</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ke</t>
   </si>
   <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feminino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Me</t>
-  </si>
-  <si>
     <t xml:space="preserve">Within this district</t>
   </si>
   <si>
@@ -2562,6 +2562,15 @@
     <t xml:space="preserve">Jua linapochomoza</t>
   </si>
   <si>
+    <t xml:space="preserve">After sunrise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depois do nascer do sol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baada ya jua kuchomoza</t>
+  </si>
+  <si>
     <t xml:space="preserve">Antes do pôr-do-sol</t>
   </si>
   <si>
@@ -4050,7 +4059,7 @@
     <t xml:space="preserve">17b. Mshiriki huyu alifanyiwa kipimo cha malaria?</t>
   </si>
   <si>
-    <t xml:space="preserve">ind_q17b1</t>
+    <t xml:space="preserve">ind_q17bi</t>
   </si>
   <si>
     <t xml:space="preserve">17b(i). [If yes] Result of the malaria test</t>
@@ -4107,7 +4116,7 @@
     <t xml:space="preserve">19. O participante tem comichão? (Assinalar todas as opções que se apliquem)</t>
   </si>
   <si>
-    <t xml:space="preserve">19. Mshirika huyu anawashwa? (chagua yote yatakayo husika)</t>
+    <t xml:space="preserve">19. Mshiriki huyu anawashwa? (chagua yote yatakayo husika)</t>
   </si>
   <si>
     <t xml:space="preserve">ind_q20</t>
@@ -4529,6 +4538,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Cascadia mono semilight"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4563,13 +4579,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Cascadia mono semilight"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -4662,7 +4671,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -4671,15 +4680,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4688,6 +4693,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4715,23 +4724,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4743,7 +4752,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Bad" xfId="20"/>
+    <cellStyle name="Bad 1" xfId="20"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -4849,11 +4858,11 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -5900,11 +5909,11 @@
   </sheetPr>
   <dimension ref="A1:Q1016"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
@@ -7387,13 +7396,13 @@
   </sheetPr>
   <dimension ref="A1:Y1011"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C90" activeCellId="0" sqref="C90"/>
+      <selection pane="bottomLeft" activeCell="B213" activeCellId="0" sqref="B213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -11179,11 +11188,11 @@
   </sheetPr>
   <dimension ref="A1:Y763"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -29607,11 +29616,11 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.04"/>
@@ -30745,15 +30754,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D354"/>
+  <dimension ref="A1:D355"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B217" activeCellId="0" sqref="B217"/>
+      <selection pane="bottomLeft" activeCell="D82" activeCellId="0" sqref="D82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="35.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="13" width="37.56"/>
@@ -33002,153 +33011,153 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="13" t="s">
-        <v>270</v>
+        <v>845</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>270</v>
+        <v>845</v>
       </c>
       <c r="C162" s="13" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D162" s="13" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C163" s="13" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D163" s="13" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C164" s="13" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D164" s="13" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C165" s="13" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D165" s="13" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C166" s="13" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D166" s="13" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="13" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C167" s="13" t="s">
-        <v>278</v>
+        <v>856</v>
       </c>
       <c r="D167" s="13" t="s">
-        <v>278</v>
+        <v>857</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C168" s="13" t="s">
-        <v>855</v>
+        <v>278</v>
       </c>
       <c r="D168" s="13" t="s">
-        <v>856</v>
+        <v>278</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C169" s="13" t="s">
-        <v>280</v>
+        <v>858</v>
       </c>
       <c r="D169" s="13" t="s">
-        <v>280</v>
+        <v>859</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>857</v>
+        <v>280</v>
       </c>
       <c r="C170" s="13" t="s">
-        <v>858</v>
+        <v>280</v>
       </c>
       <c r="D170" s="13" t="s">
-        <v>859</v>
+        <v>280</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>282</v>
+        <v>860</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>282</v>
+        <v>861</v>
       </c>
       <c r="D171" s="13" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>861</v>
+        <v>282</v>
       </c>
       <c r="C172" s="13" t="s">
-        <v>862</v>
+        <v>282</v>
       </c>
       <c r="D172" s="13" t="s">
         <v>863</v>
@@ -33156,94 +33165,94 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>284</v>
+        <v>864</v>
       </c>
       <c r="C173" s="13" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="D173" s="13" t="s">
-        <v>284</v>
+        <v>866</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C174" s="13" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D174" s="13" t="s">
-        <v>866</v>
+        <v>284</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C175" s="13" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D175" s="13" t="s">
-        <v>286</v>
+        <v>869</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C176" s="13" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="D176" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="13" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>869</v>
+        <v>287</v>
       </c>
       <c r="C177" s="13" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D177" s="13" t="s">
-        <v>871</v>
+        <v>287</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>290</v>
+        <v>872</v>
       </c>
       <c r="C178" s="13" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D178" s="13" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>874</v>
+        <v>290</v>
       </c>
       <c r="C179" s="13" t="s">
         <v>875</v>
@@ -33254,38 +33263,38 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>292</v>
+        <v>877</v>
       </c>
       <c r="C180" s="13" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="D180" s="13" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C181" s="13" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="D181" s="13" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>881</v>
+        <v>293</v>
       </c>
       <c r="C182" s="13" t="s">
         <v>882</v>
@@ -33296,24 +33305,24 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>295</v>
+        <v>884</v>
       </c>
       <c r="C183" s="13" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D183" s="13" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>886</v>
+        <v>295</v>
       </c>
       <c r="C184" s="13" t="s">
         <v>887</v>
@@ -33324,7 +33333,7 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B185" s="13" t="s">
         <v>889</v>
@@ -33338,7 +33347,7 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B186" s="13" t="s">
         <v>892</v>
@@ -33352,7 +33361,7 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B187" s="13" t="s">
         <v>895</v>
@@ -33366,7 +33375,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B188" s="13" t="s">
         <v>898</v>
@@ -33380,7 +33389,7 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B189" s="13" t="s">
         <v>901</v>
@@ -33394,7 +33403,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B190" s="13" t="s">
         <v>904</v>
@@ -33406,247 +33415,247 @@
         <v>906</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="13" t="s">
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B191" s="13" t="s">
         <v>907</v>
       </c>
-      <c r="B192" s="13" t="s">
+      <c r="C191" s="13" t="s">
         <v>908</v>
       </c>
-      <c r="C192" s="13" t="s">
+      <c r="D191" s="13" t="s">
         <v>909</v>
-      </c>
-      <c r="D192" s="13" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="13" t="s">
+        <v>910</v>
+      </c>
+      <c r="B193" s="13" t="s">
         <v>911</v>
       </c>
-      <c r="B193" s="13" t="s">
+      <c r="C193" s="13" t="s">
         <v>912</v>
       </c>
-      <c r="C193" s="13" t="s">
+      <c r="D193" s="13" t="s">
         <v>913</v>
-      </c>
-      <c r="D193" s="13" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="13" t="s">
+        <v>914</v>
+      </c>
+      <c r="B194" s="13" t="s">
         <v>915</v>
       </c>
-      <c r="B194" s="13" t="s">
+      <c r="C194" s="13" t="s">
         <v>916</v>
       </c>
-      <c r="C194" s="13" t="s">
+      <c r="D194" s="13" t="s">
         <v>917</v>
-      </c>
-      <c r="D194" s="13" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="13" t="s">
+        <v>918</v>
+      </c>
+      <c r="B195" s="13" t="s">
         <v>919</v>
       </c>
-      <c r="B195" s="13" t="s">
+      <c r="C195" s="13" t="s">
         <v>920</v>
       </c>
-      <c r="C195" s="13" t="s">
+      <c r="D195" s="13" t="s">
         <v>921</v>
-      </c>
-      <c r="D195" s="13" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="13" t="s">
+        <v>922</v>
+      </c>
+      <c r="B196" s="13" t="s">
         <v>923</v>
       </c>
-      <c r="B196" s="13" t="s">
+      <c r="C196" s="13" t="s">
         <v>924</v>
       </c>
-      <c r="C196" s="13" t="s">
+      <c r="D196" s="13" t="s">
         <v>925</v>
       </c>
-      <c r="D196" s="13" t="s">
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="13" t="s">
         <v>926</v>
       </c>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="13" t="s">
+      <c r="B197" s="13" t="s">
         <v>927</v>
       </c>
-      <c r="B198" s="13" t="s">
+      <c r="C197" s="13" t="s">
         <v>928</v>
       </c>
-      <c r="C198" s="13" t="s">
+      <c r="D197" s="13" t="s">
         <v>929</v>
-      </c>
-      <c r="D198" s="13" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="13" t="s">
+        <v>930</v>
+      </c>
+      <c r="B199" s="13" t="s">
         <v>931</v>
       </c>
-      <c r="B199" s="13" t="s">
+      <c r="C199" s="13" t="s">
         <v>932</v>
       </c>
-      <c r="C199" s="13" t="s">
+      <c r="D199" s="13" t="s">
         <v>933</v>
-      </c>
-      <c r="D199" s="13" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="13" t="s">
+        <v>934</v>
+      </c>
+      <c r="B200" s="13" t="s">
         <v>935</v>
       </c>
-      <c r="B200" s="13" t="s">
+      <c r="C200" s="13" t="s">
         <v>936</v>
       </c>
-      <c r="C200" s="13" t="s">
+      <c r="D200" s="13" t="s">
         <v>937</v>
-      </c>
-      <c r="D200" s="13" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="B201" s="13" t="s">
         <v>939</v>
       </c>
-      <c r="B201" s="13" t="s">
+      <c r="C201" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="C201" s="13" t="s">
+      <c r="D201" s="13" t="s">
         <v>941</v>
-      </c>
-      <c r="D201" s="13" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="13" t="s">
+        <v>942</v>
+      </c>
+      <c r="B202" s="13" t="s">
         <v>943</v>
       </c>
-      <c r="B202" s="13" t="s">
+      <c r="C202" s="13" t="s">
         <v>944</v>
       </c>
-      <c r="C202" s="13" t="s">
+      <c r="D202" s="13" t="s">
         <v>945</v>
-      </c>
-      <c r="D202" s="13" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="13" t="s">
+        <v>946</v>
+      </c>
+      <c r="B203" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="B203" s="13" t="s">
+      <c r="C203" s="13" t="s">
         <v>948</v>
       </c>
-      <c r="C203" s="13" t="s">
+      <c r="D203" s="13" t="s">
         <v>949</v>
-      </c>
-      <c r="D203" s="13" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="13" t="s">
+        <v>950</v>
+      </c>
+      <c r="B204" s="13" t="s">
         <v>951</v>
       </c>
-      <c r="B204" s="13" t="s">
+      <c r="C204" s="13" t="s">
         <v>952</v>
       </c>
-      <c r="C204" s="13" t="s">
+      <c r="D204" s="13" t="s">
         <v>953</v>
       </c>
-      <c r="D204" s="13" t="s">
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="13" t="s">
         <v>954</v>
       </c>
-    </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B206" s="13" t="s">
+      <c r="B205" s="13" t="s">
         <v>955</v>
       </c>
-      <c r="C206" s="13" t="s">
-        <v>593</v>
-      </c>
-      <c r="D206" s="13" t="s">
-        <v>594</v>
+      <c r="C205" s="13" t="s">
+        <v>956</v>
+      </c>
+      <c r="D205" s="13" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="13" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C207" s="13" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="D207" s="13" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="C208" s="13" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="D208" s="13" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="13" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C209" s="13" t="s">
-        <v>959</v>
+        <v>607</v>
       </c>
       <c r="D209" s="13" t="s">
-        <v>960</v>
+        <v>608</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B210" s="13" t="s">
         <v>961</v>
       </c>
-      <c r="B210" s="13" t="s">
+      <c r="C210" s="13" t="s">
         <v>962</v>
       </c>
-      <c r="C210" s="13" t="s">
+      <c r="D210" s="13" t="s">
         <v>963</v>
-      </c>
-      <c r="D210" s="13" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="13" t="s">
-        <v>323</v>
+        <v>964</v>
       </c>
       <c r="B211" s="13" t="s">
         <v>965</v>
@@ -33660,227 +33669,227 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B212" s="13" t="s">
         <v>968</v>
       </c>
-      <c r="B212" s="13" t="s">
+      <c r="C212" s="13" t="s">
         <v>969</v>
       </c>
-      <c r="C212" s="13" t="s">
+      <c r="D212" s="13" t="s">
         <v>970</v>
-      </c>
-      <c r="D212" s="13" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="13" t="s">
+        <v>971</v>
+      </c>
+      <c r="B213" s="13" t="s">
         <v>972</v>
       </c>
-      <c r="B213" s="13" t="s">
+      <c r="C213" s="13" t="s">
         <v>973</v>
       </c>
-      <c r="C213" s="13" t="s">
+      <c r="D213" s="13" t="s">
         <v>974</v>
-      </c>
-      <c r="D213" s="13" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="13" t="s">
+        <v>975</v>
+      </c>
+      <c r="B214" s="13" t="s">
         <v>976</v>
       </c>
-      <c r="B214" s="13" t="s">
+      <c r="C214" s="13" t="s">
         <v>977</v>
       </c>
-      <c r="C214" s="13" t="s">
+      <c r="D214" s="13" t="s">
         <v>978</v>
       </c>
-      <c r="D214" s="13" t="s">
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="13" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="215" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="13" t="s">
+      <c r="B215" s="13" t="s">
         <v>980</v>
       </c>
-      <c r="B215" s="13" t="s">
+      <c r="C215" s="13" t="s">
         <v>981</v>
       </c>
-      <c r="C215" s="14" t="s">
+      <c r="D215" s="13" t="s">
         <v>982</v>
-      </c>
-      <c r="D215" s="14" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="13" t="s">
+        <v>983</v>
+      </c>
+      <c r="B216" s="13" t="s">
         <v>984</v>
       </c>
-      <c r="B216" s="13" t="s">
+      <c r="C216" s="14" t="s">
         <v>985</v>
       </c>
-      <c r="C216" s="14" t="s">
+      <c r="D216" s="14" t="s">
         <v>986</v>
       </c>
-      <c r="D216" s="14" t="s">
+    </row>
+    <row r="217" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="13" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="13" t="s">
+      <c r="B217" s="13" t="s">
         <v>988</v>
       </c>
-      <c r="B217" s="13" t="s">
+      <c r="C217" s="14" t="s">
         <v>989</v>
       </c>
-      <c r="C217" s="15"/>
-      <c r="D217" s="15"/>
+      <c r="D217" s="14" t="s">
+        <v>990</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="13" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>991</v>
-      </c>
-      <c r="C218" s="13" t="s">
         <v>992</v>
       </c>
-      <c r="D218" s="13" t="s">
-        <v>993</v>
-      </c>
+      <c r="C218" s="15"/>
+      <c r="D218" s="15"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="13" t="s">
+        <v>993</v>
+      </c>
+      <c r="B219" s="13" t="s">
         <v>994</v>
       </c>
-      <c r="B219" s="13" t="s">
+      <c r="C219" s="13" t="s">
         <v>995</v>
       </c>
-      <c r="C219" s="13" t="s">
+      <c r="D219" s="13" t="s">
         <v>996</v>
-      </c>
-      <c r="D219" s="13" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="13" t="s">
+        <v>997</v>
+      </c>
+      <c r="B220" s="13" t="s">
         <v>998</v>
       </c>
-      <c r="B220" s="13" t="s">
+      <c r="C220" s="13" t="s">
         <v>999</v>
       </c>
-      <c r="C220" s="13" t="s">
+      <c r="D220" s="13" t="s">
         <v>1000</v>
-      </c>
-      <c r="D220" s="13" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="13" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B221" s="13" t="s">
         <v>1002</v>
       </c>
-      <c r="B221" s="13" t="s">
+      <c r="C221" s="13" t="s">
         <v>1003</v>
       </c>
-      <c r="C221" s="13" t="s">
+      <c r="D221" s="13" t="s">
         <v>1004</v>
-      </c>
-      <c r="D221" s="13" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="13" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B222" s="13" t="s">
         <v>1006</v>
       </c>
-      <c r="B222" s="13" t="s">
+      <c r="C222" s="13" t="s">
         <v>1007</v>
       </c>
-      <c r="C222" s="14" t="s">
+      <c r="D222" s="13" t="s">
         <v>1008</v>
-      </c>
-      <c r="D222" s="14" t="s">
-        <v>1009</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B223" s="13" t="s">
         <v>1010</v>
       </c>
-      <c r="B223" s="13" t="s">
+      <c r="C223" s="14" t="s">
         <v>1011</v>
       </c>
-      <c r="C223" s="13" t="s">
+      <c r="D223" s="14" t="s">
         <v>1012</v>
-      </c>
-      <c r="D223" s="13" t="s">
-        <v>1013</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="13" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B224" s="13" t="s">
         <v>1014</v>
-      </c>
-      <c r="B224" s="13" t="s">
-        <v>1015</v>
       </c>
       <c r="C224" s="13" t="s">
         <v>1015</v>
       </c>
       <c r="D224" s="13" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="13" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>1017</v>
-      </c>
-      <c r="C225" s="14" t="s">
         <v>1018</v>
       </c>
-      <c r="D225" s="14" t="s">
+      <c r="C225" s="13" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D225" s="13" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="13" t="s">
         <v>1019</v>
       </c>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="13" t="s">
+      <c r="B226" s="13" t="s">
         <v>1020</v>
       </c>
-      <c r="B226" s="13" t="s">
+      <c r="C226" s="14" t="s">
         <v>1021</v>
       </c>
-      <c r="C226" s="13" t="s">
+      <c r="D226" s="14" t="s">
         <v>1022</v>
-      </c>
-      <c r="D226" s="13" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="13" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B227" s="13" t="s">
         <v>1024</v>
       </c>
-      <c r="B227" s="13" t="s">
+      <c r="C227" s="13" t="s">
         <v>1025</v>
       </c>
-      <c r="C227" s="13" t="s">
+      <c r="D227" s="13" t="s">
         <v>1026</v>
-      </c>
-      <c r="D227" s="13" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="13" t="s">
-        <v>27</v>
+        <v>1027</v>
       </c>
       <c r="B228" s="13" t="s">
         <v>1028</v>
@@ -33894,147 +33903,147 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B229" s="13" t="s">
         <v>1031</v>
       </c>
-      <c r="B229" s="13" t="s">
+      <c r="C229" s="13" t="s">
         <v>1032</v>
       </c>
-      <c r="C229" s="13" t="s">
+      <c r="D229" s="13" t="s">
         <v>1033</v>
-      </c>
-      <c r="D229" s="13" t="s">
-        <v>1034</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B230" s="13" t="s">
         <v>1035</v>
       </c>
-      <c r="B230" s="13" t="s">
+      <c r="C230" s="13" t="s">
         <v>1036</v>
       </c>
-      <c r="C230" s="13" t="s">
+      <c r="D230" s="13" t="s">
         <v>1037</v>
-      </c>
-      <c r="D230" s="13" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B231" s="13" t="s">
         <v>1039</v>
       </c>
-      <c r="B231" s="13" t="s">
+      <c r="C231" s="13" t="s">
         <v>1040</v>
       </c>
-      <c r="C231" s="13" t="s">
+      <c r="D231" s="13" t="s">
         <v>1041</v>
-      </c>
-      <c r="D231" s="13" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B232" s="13" t="s">
         <v>1043</v>
       </c>
-      <c r="B232" s="13" t="s">
+      <c r="C232" s="13" t="s">
         <v>1044</v>
       </c>
-      <c r="C232" s="13" t="s">
+      <c r="D232" s="13" t="s">
         <v>1045</v>
-      </c>
-      <c r="D232" s="13" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="13" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B233" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="B233" s="13" t="s">
+      <c r="C233" s="13" t="s">
         <v>1048</v>
       </c>
-      <c r="C233" s="13" t="s">
+      <c r="D233" s="13" t="s">
         <v>1049</v>
-      </c>
-      <c r="D233" s="13" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B234" s="13" t="s">
         <v>1051</v>
       </c>
-      <c r="B234" s="13" t="s">
+      <c r="C234" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="C234" s="13" t="s">
+      <c r="D234" s="13" t="s">
         <v>1053</v>
-      </c>
-      <c r="D234" s="13" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="13" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B235" s="13" t="s">
         <v>1055</v>
       </c>
-      <c r="B235" s="13" t="s">
+      <c r="C235" s="13" t="s">
         <v>1056</v>
       </c>
-      <c r="C235" s="13" t="s">
+      <c r="D235" s="13" t="s">
         <v>1057</v>
-      </c>
-      <c r="D235" s="13" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="13" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B236" s="13" t="s">
         <v>1059</v>
       </c>
-      <c r="B236" s="13" t="s">
+      <c r="C236" s="13" t="s">
         <v>1060</v>
       </c>
-      <c r="C236" s="14" t="s">
+      <c r="D236" s="13" t="s">
         <v>1061</v>
       </c>
-      <c r="D236" s="14" t="s">
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="13" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="237" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="13" t="s">
+      <c r="B237" s="13" t="s">
         <v>1063</v>
       </c>
-      <c r="B237" s="13" t="s">
+      <c r="C237" s="14" t="s">
         <v>1064</v>
       </c>
-      <c r="C237" s="14" t="s">
+      <c r="D237" s="14" t="s">
         <v>1065</v>
       </c>
-      <c r="D237" s="14" t="s">
+    </row>
+    <row r="238" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="13" t="s">
         <v>1066</v>
       </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="13" t="s">
+      <c r="B238" s="13" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C238" s="14" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D238" s="14" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="B239" s="13" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C239" s="14" t="s">
-        <v>1068</v>
-      </c>
-      <c r="D239" s="14" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A240" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="B240" s="13" t="s">
         <v>1070</v>
@@ -34046,23 +34055,23 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B241" s="13" t="s">
         <v>1073</v>
       </c>
-      <c r="C241" s="13" t="s">
+      <c r="C241" s="14" t="s">
         <v>1074</v>
       </c>
-      <c r="D241" s="13" t="s">
+      <c r="D241" s="14" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="13" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B242" s="13" t="s">
         <v>1076</v>
@@ -34076,7 +34085,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B243" s="13" t="s">
         <v>1079</v>
@@ -34088,79 +34097,79 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B244" s="13" t="s">
         <v>1082</v>
       </c>
-      <c r="B244" s="13" t="s">
+      <c r="C244" s="13" t="s">
         <v>1083</v>
       </c>
-      <c r="C244" s="14" t="s">
+      <c r="D244" s="13" t="s">
         <v>1084</v>
-      </c>
-      <c r="D244" s="14" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B245" s="13" t="s">
         <v>1086</v>
       </c>
-      <c r="B245" s="13" t="s">
+      <c r="C245" s="14" t="s">
         <v>1087</v>
       </c>
-      <c r="C245" s="14" t="s">
+      <c r="D245" s="14" t="s">
         <v>1088</v>
-      </c>
-      <c r="D245" s="14" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="13" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B246" s="13" t="s">
         <v>1090</v>
       </c>
-      <c r="B246" s="13" t="s">
+      <c r="C246" s="14" t="s">
         <v>1091</v>
       </c>
-      <c r="C246" s="14" t="s">
+      <c r="D246" s="14" t="s">
         <v>1092</v>
       </c>
-      <c r="D246" s="14" t="s">
+    </row>
+    <row r="247" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="13" t="s">
         <v>1093</v>
       </c>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="13" t="s">
+      <c r="B247" s="13" t="s">
         <v>1094</v>
       </c>
-      <c r="B247" s="13" t="s">
+      <c r="C247" s="14" t="s">
         <v>1095</v>
       </c>
-      <c r="C247" s="13" t="s">
+      <c r="D247" s="14" t="s">
         <v>1096</v>
       </c>
-      <c r="D247" s="13" t="s">
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="13" t="s">
         <v>1097</v>
       </c>
-    </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B250" s="13" t="s">
+      <c r="B248" s="13" t="s">
         <v>1098</v>
       </c>
-      <c r="C250" s="13" t="s">
+      <c r="C248" s="13" t="s">
         <v>1099</v>
       </c>
-      <c r="D250" s="13" t="s">
+      <c r="D248" s="13" t="s">
         <v>1100</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B251" s="13" t="s">
         <v>1101</v>
@@ -34174,7 +34183,7 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B252" s="13" t="s">
         <v>1104</v>
@@ -34188,7 +34197,7 @@
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="13" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B253" s="13" t="s">
         <v>1107</v>
@@ -34202,7 +34211,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B254" s="13" t="s">
         <v>1110</v>
@@ -34216,7 +34225,7 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B255" s="13" t="s">
         <v>1113</v>
@@ -34230,7 +34239,7 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B256" s="13" t="s">
         <v>1116</v>
@@ -34244,178 +34253,178 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B257" s="13" t="s">
         <v>1119</v>
       </c>
-      <c r="B257" s="13" t="s">
+      <c r="C257" s="13" t="s">
         <v>1120</v>
       </c>
-      <c r="C257" s="13" t="s">
+      <c r="D257" s="13" t="s">
         <v>1121</v>
-      </c>
-      <c r="D257" s="13" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="13" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B258" s="13" t="s">
         <v>1123</v>
       </c>
-      <c r="B258" s="13" t="s">
+      <c r="C258" s="13" t="s">
         <v>1124</v>
       </c>
-      <c r="C258" s="13" t="s">
+      <c r="D258" s="13" t="s">
         <v>1125</v>
-      </c>
-      <c r="D258" s="13" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="13" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B259" s="13" t="s">
         <v>1127</v>
       </c>
-      <c r="B259" s="13" t="s">
+      <c r="C259" s="13" t="s">
         <v>1128</v>
       </c>
-      <c r="C259" s="13" t="s">
+      <c r="D259" s="13" t="s">
         <v>1129</v>
-      </c>
-      <c r="D259" s="13" t="s">
-        <v>1130</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="13" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B260" s="13" t="s">
         <v>1131</v>
       </c>
-      <c r="B260" s="13" t="s">
+      <c r="C260" s="13" t="s">
         <v>1132</v>
       </c>
-      <c r="C260" s="13" t="s">
+      <c r="D260" s="13" t="s">
         <v>1133</v>
-      </c>
-      <c r="D260" s="13" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="13" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B261" s="13" t="s">
         <v>1135</v>
       </c>
-      <c r="B261" s="13" t="s">
+      <c r="C261" s="13" t="s">
         <v>1136</v>
       </c>
-      <c r="C261" s="13" t="s">
+      <c r="D261" s="13" t="s">
         <v>1137</v>
-      </c>
-      <c r="D261" s="13" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="13" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B262" s="13" t="s">
         <v>1139</v>
       </c>
-      <c r="B262" s="13" t="s">
+      <c r="C262" s="13" t="s">
         <v>1140</v>
       </c>
-      <c r="C262" s="13" t="s">
+      <c r="D262" s="13" t="s">
         <v>1141</v>
-      </c>
-      <c r="D262" s="13" t="s">
-        <v>1142</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="13" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B263" s="13" t="s">
         <v>1143</v>
       </c>
-      <c r="B263" s="13" t="s">
+      <c r="C263" s="13" t="s">
         <v>1144</v>
       </c>
-      <c r="C263" s="13" t="s">
+      <c r="D263" s="13" t="s">
         <v>1145</v>
-      </c>
-      <c r="D263" s="13" t="s">
-        <v>1146</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="13" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B264" s="13" t="s">
         <v>1147</v>
       </c>
-      <c r="B264" s="13" t="s">
+      <c r="C264" s="13" t="s">
         <v>1148</v>
       </c>
-      <c r="C264" s="13" t="s">
+      <c r="D264" s="13" t="s">
         <v>1149</v>
-      </c>
-      <c r="D264" s="13" t="s">
-        <v>1150</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="13" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B265" s="13" t="s">
         <v>1151</v>
       </c>
-      <c r="B265" s="13" t="s">
+      <c r="C265" s="13" t="s">
         <v>1152</v>
       </c>
-      <c r="C265" s="13" t="s">
+      <c r="D265" s="13" t="s">
         <v>1153</v>
-      </c>
-      <c r="D265" s="13" t="s">
-        <v>1154</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="13" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B266" s="13" t="s">
         <v>1155</v>
       </c>
-      <c r="B266" s="13" t="s">
+      <c r="C266" s="13" t="s">
         <v>1156</v>
       </c>
-      <c r="C266" s="13" t="s">
+      <c r="D266" s="13" t="s">
         <v>1157</v>
-      </c>
-      <c r="D266" s="13" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="13" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B267" s="13" t="s">
         <v>1159</v>
       </c>
-      <c r="B267" s="13" t="s">
+      <c r="C267" s="13" t="s">
         <v>1160</v>
       </c>
-      <c r="C267" s="13" t="s">
+      <c r="D267" s="13" t="s">
         <v>1161</v>
-      </c>
-      <c r="D267" s="13" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="13" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B268" s="13" t="s">
         <v>1163</v>
       </c>
-      <c r="B268" s="13" t="s">
+      <c r="C268" s="13" t="s">
         <v>1164</v>
       </c>
-      <c r="C268" s="13" t="s">
+      <c r="D268" s="13" t="s">
         <v>1165</v>
-      </c>
-      <c r="D268" s="13" t="s">
-        <v>1166</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="13" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B269" s="13" t="s">
         <v>1167</v>
-      </c>
-      <c r="B269" s="13" t="s">
-        <v>1116</v>
       </c>
       <c r="C269" s="13" t="s">
         <v>1168</v>
@@ -34429,1165 +34438,1179 @@
         <v>1170</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>1171</v>
+        <v>1119</v>
       </c>
       <c r="C270" s="13" t="s">
         <v>1171</v>
       </c>
       <c r="D270" s="13" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="13" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B271" s="13" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="C271" s="13" t="s">
         <v>1174</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="13" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B272" s="13" t="s">
         <v>1176</v>
       </c>
-      <c r="B272" s="13" t="s">
+      <c r="C272" s="13" t="s">
         <v>1177</v>
       </c>
-      <c r="C272" s="13" t="s">
+      <c r="D272" s="13" t="s">
         <v>1178</v>
-      </c>
-      <c r="D272" s="13" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="13" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B273" s="13" t="s">
         <v>1180</v>
       </c>
-      <c r="B273" s="13" t="s">
+      <c r="C273" s="13" t="s">
         <v>1181</v>
       </c>
-      <c r="C273" s="13" t="s">
+      <c r="D273" s="13" t="s">
         <v>1182</v>
-      </c>
-      <c r="D273" s="13" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="13" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B274" s="13" t="s">
         <v>1184</v>
       </c>
-      <c r="B274" s="13" t="s">
+      <c r="C274" s="13" t="s">
         <v>1185</v>
       </c>
-      <c r="C274" s="13" t="s">
+      <c r="D274" s="13" t="s">
         <v>1186</v>
-      </c>
-      <c r="D274" s="13" t="s">
-        <v>1187</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="13" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B275" s="13" t="s">
         <v>1188</v>
       </c>
-      <c r="B275" s="13" t="s">
+      <c r="C275" s="13" t="s">
         <v>1189</v>
       </c>
-      <c r="C275" s="13" t="s">
+      <c r="D275" s="13" t="s">
         <v>1190</v>
-      </c>
-      <c r="D275" s="13" t="s">
-        <v>1191</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="13" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B276" s="13" t="s">
         <v>1192</v>
       </c>
-      <c r="B276" s="13" t="s">
+      <c r="C276" s="13" t="s">
         <v>1193</v>
       </c>
-      <c r="C276" s="13" t="s">
+      <c r="D276" s="13" t="s">
         <v>1194</v>
-      </c>
-      <c r="D276" s="13" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="13" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B277" s="13" t="s">
         <v>1196</v>
       </c>
-      <c r="B277" s="13" t="s">
-        <v>1116</v>
-      </c>
       <c r="C277" s="13" t="s">
-        <v>1168</v>
+        <v>1197</v>
       </c>
       <c r="D277" s="13" t="s">
-        <v>1169</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="13" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>1198</v>
+        <v>1119</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>1199</v>
+        <v>1171</v>
       </c>
       <c r="D278" s="13" t="s">
-        <v>1200</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="13" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B279" s="13" t="s">
         <v>1201</v>
       </c>
-      <c r="B279" s="13" t="s">
+      <c r="C279" s="13" t="s">
         <v>1202</v>
       </c>
-      <c r="C279" s="13" t="s">
+      <c r="D279" s="13" t="s">
         <v>1203</v>
-      </c>
-      <c r="D279" s="13" t="s">
-        <v>1204</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="13" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B280" s="13" t="s">
         <v>1205</v>
       </c>
-      <c r="B280" s="13" t="s">
+      <c r="C280" s="13" t="s">
         <v>1206</v>
       </c>
-      <c r="C280" s="13" t="s">
+      <c r="D280" s="13" t="s">
         <v>1207</v>
-      </c>
-      <c r="D280" s="13" t="s">
-        <v>1208</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="13" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B281" s="13" t="s">
         <v>1209</v>
       </c>
-      <c r="B281" s="13" t="s">
+      <c r="C281" s="13" t="s">
         <v>1210</v>
       </c>
-      <c r="C281" s="13" t="s">
+      <c r="D281" s="13" t="s">
         <v>1211</v>
-      </c>
-      <c r="D281" s="13" t="s">
-        <v>1212</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="13" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B282" s="13" t="s">
         <v>1213</v>
       </c>
-      <c r="B282" s="13" t="s">
+      <c r="C282" s="13" t="s">
         <v>1214</v>
       </c>
-      <c r="C282" s="13" t="s">
+      <c r="D282" s="13" t="s">
         <v>1215</v>
-      </c>
-      <c r="D282" s="13" t="s">
-        <v>1216</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="13" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B283" s="13" t="s">
         <v>1217</v>
       </c>
-      <c r="B283" s="13" t="s">
+      <c r="C283" s="13" t="s">
         <v>1218</v>
       </c>
-      <c r="C283" s="13" t="s">
+      <c r="D283" s="13" t="s">
         <v>1219</v>
-      </c>
-      <c r="D283" s="13" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="13" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B284" s="13" t="s">
         <v>1221</v>
       </c>
-      <c r="B284" s="13" t="s">
+      <c r="C284" s="13" t="s">
         <v>1222</v>
       </c>
-      <c r="C284" s="13" t="s">
+      <c r="D284" s="13" t="s">
         <v>1223</v>
-      </c>
-      <c r="D284" s="13" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="13" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B285" s="13" t="s">
         <v>1225</v>
       </c>
-      <c r="B285" s="13" t="s">
+      <c r="C285" s="13" t="s">
         <v>1226</v>
       </c>
-      <c r="C285" s="13" t="s">
+      <c r="D285" s="13" t="s">
         <v>1227</v>
-      </c>
-      <c r="D285" s="13" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="13" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B286" s="13" t="s">
         <v>1229</v>
       </c>
-      <c r="B286" s="13" t="s">
+      <c r="C286" s="13" t="s">
         <v>1230</v>
       </c>
-      <c r="C286" s="13" t="s">
+      <c r="D286" s="13" t="s">
         <v>1231</v>
-      </c>
-      <c r="D286" s="13" t="s">
-        <v>1232</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="13" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B287" s="13" t="s">
         <v>1233</v>
       </c>
-      <c r="B287" s="13" t="s">
+      <c r="C287" s="13" t="s">
         <v>1234</v>
       </c>
-      <c r="C287" s="13" t="s">
+      <c r="D287" s="13" t="s">
         <v>1235</v>
-      </c>
-      <c r="D287" s="13" t="s">
-        <v>1236</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="13" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B288" s="13" t="s">
         <v>1237</v>
       </c>
-      <c r="B288" s="13" t="s">
+      <c r="C288" s="13" t="s">
         <v>1238</v>
       </c>
-      <c r="C288" s="13" t="s">
+      <c r="D288" s="13" t="s">
         <v>1239</v>
-      </c>
-      <c r="D288" s="13" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="13" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B289" s="13" t="s">
         <v>1241</v>
       </c>
-      <c r="B289" s="13" t="s">
+      <c r="C289" s="13" t="s">
         <v>1242</v>
       </c>
-      <c r="C289" s="13" t="s">
+      <c r="D289" s="13" t="s">
         <v>1243</v>
-      </c>
-      <c r="D289" s="13" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="13" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B290" s="13" t="s">
         <v>1245</v>
       </c>
-      <c r="B290" s="13" t="s">
+      <c r="C290" s="13" t="s">
         <v>1246</v>
       </c>
-      <c r="C290" s="13" t="s">
+      <c r="D290" s="13" t="s">
         <v>1247</v>
       </c>
-      <c r="D290" s="13" t="s">
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="13" t="s">
         <v>1248</v>
       </c>
-    </row>
-    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="13" t="s">
+      <c r="B291" s="13" t="s">
         <v>1249</v>
       </c>
-      <c r="B292" s="13" t="s">
+      <c r="C291" s="13" t="s">
         <v>1250</v>
       </c>
-      <c r="C292" s="13" t="s">
+      <c r="D291" s="13" t="s">
         <v>1251</v>
-      </c>
-      <c r="D292" s="13" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="13" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B293" s="13" t="s">
         <v>1253</v>
       </c>
-      <c r="B293" s="13" t="s">
+      <c r="C293" s="13" t="s">
         <v>1254</v>
       </c>
-      <c r="C293" s="13" t="s">
+      <c r="D293" s="13" t="s">
         <v>1255</v>
-      </c>
-      <c r="D293" s="13" t="s">
-        <v>1256</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="13" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B294" s="13" t="s">
         <v>1257</v>
       </c>
-      <c r="B294" s="13" t="s">
+      <c r="C294" s="13" t="s">
         <v>1258</v>
       </c>
-      <c r="C294" s="13" t="s">
+      <c r="D294" s="13" t="s">
         <v>1259</v>
-      </c>
-      <c r="D294" s="13" t="s">
-        <v>1260</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="13" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B295" s="13" t="s">
         <v>1261</v>
       </c>
-      <c r="B295" s="13" t="s">
+      <c r="C295" s="13" t="s">
         <v>1262</v>
       </c>
-      <c r="C295" s="13" t="s">
+      <c r="D295" s="13" t="s">
         <v>1263</v>
-      </c>
-      <c r="D295" s="13" t="s">
-        <v>1264</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="13" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B296" s="13" t="s">
         <v>1265</v>
       </c>
-      <c r="B296" s="13" t="s">
+      <c r="C296" s="13" t="s">
         <v>1266</v>
       </c>
-      <c r="C296" s="13" t="s">
+      <c r="D296" s="13" t="s">
         <v>1267</v>
-      </c>
-      <c r="D296" s="13" t="s">
-        <v>1268</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="13" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B297" s="13" t="s">
         <v>1269</v>
       </c>
-      <c r="B297" s="13" t="s">
+      <c r="C297" s="13" t="s">
         <v>1270</v>
       </c>
-      <c r="C297" s="13" t="s">
+      <c r="D297" s="13" t="s">
         <v>1271</v>
-      </c>
-      <c r="D297" s="13" t="s">
-        <v>1272</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="13" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B298" s="13" t="s">
         <v>1273</v>
       </c>
-      <c r="B298" s="13" t="s">
+      <c r="C298" s="13" t="s">
         <v>1274</v>
       </c>
-      <c r="C298" s="13" t="s">
+      <c r="D298" s="13" t="s">
         <v>1275</v>
-      </c>
-      <c r="D298" s="13" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="13" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B299" s="13" t="s">
         <v>1277</v>
       </c>
-      <c r="B299" s="13" t="s">
+      <c r="C299" s="13" t="s">
         <v>1278</v>
       </c>
-      <c r="C299" s="13" t="s">
+      <c r="D299" s="13" t="s">
         <v>1279</v>
-      </c>
-      <c r="D299" s="13" t="s">
-        <v>1280</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="13" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B300" s="13" t="s">
         <v>1281</v>
       </c>
-      <c r="B300" s="13" t="s">
+      <c r="C300" s="13" t="s">
         <v>1282</v>
       </c>
-      <c r="C300" s="13" t="s">
+      <c r="D300" s="13" t="s">
         <v>1283</v>
-      </c>
-      <c r="D300" s="13" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="13" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B301" s="13" t="s">
         <v>1285</v>
       </c>
-      <c r="B301" s="13" t="s">
+      <c r="C301" s="13" t="s">
         <v>1286</v>
       </c>
-      <c r="C301" s="13" t="s">
+      <c r="D301" s="13" t="s">
         <v>1287</v>
-      </c>
-      <c r="D301" s="13" t="s">
-        <v>1288</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="13" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B302" s="13" t="s">
         <v>1289</v>
       </c>
-      <c r="B302" s="13" t="s">
+      <c r="C302" s="13" t="s">
         <v>1290</v>
       </c>
-      <c r="C302" s="13" t="s">
+      <c r="D302" s="13" t="s">
         <v>1291</v>
-      </c>
-      <c r="D302" s="13" t="s">
-        <v>1292</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="13" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B303" s="13" t="s">
         <v>1293</v>
       </c>
-      <c r="B303" s="13" t="s">
+      <c r="C303" s="13" t="s">
         <v>1294</v>
       </c>
-      <c r="C303" s="13" t="s">
+      <c r="D303" s="13" t="s">
         <v>1295</v>
-      </c>
-      <c r="D303" s="13" t="s">
-        <v>1296</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="13" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B304" s="13" t="s">
         <v>1297</v>
       </c>
-      <c r="B304" s="13" t="s">
+      <c r="C304" s="13" t="s">
         <v>1298</v>
       </c>
-      <c r="C304" s="13" t="s">
+      <c r="D304" s="13" t="s">
         <v>1299</v>
-      </c>
-      <c r="D304" s="13" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="13" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B305" s="13" t="s">
         <v>1301</v>
       </c>
-      <c r="B305" s="13" t="s">
+      <c r="C305" s="13" t="s">
         <v>1302</v>
       </c>
-      <c r="C305" s="13" t="s">
+      <c r="D305" s="13" t="s">
         <v>1303</v>
-      </c>
-      <c r="D305" s="13" t="s">
-        <v>1304</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="13" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B306" s="13" t="s">
         <v>1305</v>
       </c>
-      <c r="B306" s="13" t="s">
+      <c r="C306" s="13" t="s">
         <v>1306</v>
       </c>
-      <c r="C306" s="13" t="s">
+      <c r="D306" s="13" t="s">
         <v>1307</v>
-      </c>
-      <c r="D306" s="13" t="s">
-        <v>1308</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="13" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B307" s="13" t="s">
         <v>1309</v>
       </c>
-      <c r="B307" s="13" t="s">
+      <c r="C307" s="13" t="s">
         <v>1310</v>
       </c>
-      <c r="C307" s="13" t="s">
+      <c r="D307" s="13" t="s">
         <v>1311</v>
-      </c>
-      <c r="D307" s="13" t="s">
-        <v>1312</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="13" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B308" s="13" t="s">
         <v>1313</v>
       </c>
-      <c r="B308" s="13" t="s">
+      <c r="C308" s="13" t="s">
         <v>1314</v>
       </c>
-      <c r="C308" s="13" t="s">
+      <c r="D308" s="13" t="s">
         <v>1315</v>
-      </c>
-      <c r="D308" s="13" t="s">
-        <v>1316</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="13" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B309" s="13" t="s">
         <v>1317</v>
       </c>
-      <c r="B309" s="13" t="s">
+      <c r="C309" s="13" t="s">
         <v>1318</v>
       </c>
-      <c r="C309" s="13" t="s">
+      <c r="D309" s="13" t="s">
         <v>1319</v>
-      </c>
-      <c r="D309" s="13" t="s">
-        <v>1320</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="13" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B310" s="13" t="s">
         <v>1321</v>
       </c>
-      <c r="B310" s="13" t="s">
+      <c r="C310" s="13" t="s">
         <v>1322</v>
       </c>
-      <c r="C310" s="13" t="s">
+      <c r="D310" s="13" t="s">
         <v>1323</v>
-      </c>
-      <c r="D310" s="13" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="13" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B311" s="13" t="s">
         <v>1325</v>
       </c>
-      <c r="B311" s="13" t="s">
+      <c r="C311" s="13" t="s">
         <v>1326</v>
       </c>
-      <c r="C311" s="13" t="s">
+      <c r="D311" s="13" t="s">
         <v>1327</v>
-      </c>
-      <c r="D311" s="13" t="s">
-        <v>1328</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="13" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B312" s="13" t="s">
         <v>1329</v>
       </c>
-      <c r="B312" s="13" t="s">
+      <c r="C312" s="13" t="s">
         <v>1330</v>
       </c>
-      <c r="C312" s="13" t="s">
+      <c r="D312" s="13" t="s">
         <v>1331</v>
-      </c>
-      <c r="D312" s="13" t="s">
-        <v>1332</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="13" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B313" s="13" t="s">
         <v>1333</v>
       </c>
-      <c r="B313" s="13" t="s">
+      <c r="C313" s="13" t="s">
         <v>1334</v>
       </c>
-      <c r="C313" s="13" t="s">
+      <c r="D313" s="13" t="s">
         <v>1335</v>
-      </c>
-      <c r="D313" s="13" t="s">
-        <v>1336</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="13" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B314" s="13" t="s">
         <v>1337</v>
       </c>
-      <c r="B314" s="13" t="s">
+      <c r="C314" s="13" t="s">
         <v>1338</v>
       </c>
-      <c r="C314" s="13" t="s">
+      <c r="D314" s="13" t="s">
         <v>1339</v>
-      </c>
-      <c r="D314" s="13" t="s">
-        <v>1340</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="13" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B315" s="13" t="s">
         <v>1341</v>
       </c>
-      <c r="B315" s="13" t="s">
+      <c r="C315" s="13" t="s">
         <v>1342</v>
       </c>
-      <c r="C315" s="13" t="s">
+      <c r="D315" s="13" t="s">
         <v>1343</v>
-      </c>
-      <c r="D315" s="13" t="s">
-        <v>1344</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="13" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B316" s="13" t="s">
         <v>1345</v>
       </c>
-      <c r="B316" s="13" t="s">
+      <c r="C316" s="13" t="s">
         <v>1346</v>
       </c>
-      <c r="C316" s="13" t="s">
+      <c r="D316" s="13" t="s">
         <v>1347</v>
-      </c>
-      <c r="D316" s="13" t="s">
-        <v>1348</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="13" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B317" s="13" t="s">
         <v>1349</v>
       </c>
-      <c r="B317" s="13" t="s">
+      <c r="C317" s="13" t="s">
         <v>1350</v>
       </c>
-      <c r="C317" s="13" t="s">
+      <c r="D317" s="13" t="s">
         <v>1351</v>
-      </c>
-      <c r="D317" s="13" t="s">
-        <v>1352</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="13" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B318" s="13" t="s">
         <v>1353</v>
       </c>
-      <c r="B318" s="13" t="s">
+      <c r="C318" s="13" t="s">
         <v>1354</v>
       </c>
-      <c r="C318" s="13" t="s">
+      <c r="D318" s="13" t="s">
         <v>1355</v>
-      </c>
-      <c r="D318" s="13" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="13" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B319" s="13" t="s">
         <v>1357</v>
       </c>
-      <c r="B319" s="13" t="s">
+      <c r="C319" s="13" t="s">
         <v>1358</v>
       </c>
-      <c r="C319" s="13" t="s">
+      <c r="D319" s="13" t="s">
         <v>1359</v>
-      </c>
-      <c r="D319" s="13" t="s">
-        <v>1360</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="13" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B320" s="13" t="s">
         <v>1361</v>
       </c>
-      <c r="B320" s="13" t="s">
+      <c r="C320" s="13" t="s">
         <v>1362</v>
       </c>
-      <c r="C320" s="13" t="s">
+      <c r="D320" s="13" t="s">
         <v>1363</v>
-      </c>
-      <c r="D320" s="13" t="s">
-        <v>1364</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="13" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B321" s="13" t="s">
         <v>1365</v>
       </c>
-      <c r="B321" s="13" t="s">
+      <c r="C321" s="13" t="s">
         <v>1366</v>
       </c>
-      <c r="C321" s="13" t="s">
+      <c r="D321" s="13" t="s">
         <v>1367</v>
-      </c>
-      <c r="D321" s="13" t="s">
-        <v>1368</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B322" s="13" t="s">
         <v>1369</v>
       </c>
-      <c r="B322" s="13" t="s">
+      <c r="C322" s="13" t="s">
         <v>1370</v>
       </c>
-      <c r="C322" s="13" t="s">
+      <c r="D322" s="13" t="s">
         <v>1371</v>
-      </c>
-      <c r="D322" s="13" t="s">
-        <v>1372</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="13" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B323" s="13" t="s">
         <v>1373</v>
       </c>
-      <c r="B323" s="13" t="s">
+      <c r="C323" s="13" t="s">
         <v>1374</v>
       </c>
-      <c r="C323" s="13" t="s">
+      <c r="D323" s="13" t="s">
         <v>1375</v>
-      </c>
-      <c r="D323" s="13" t="s">
-        <v>1376</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="13" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B324" s="13" t="s">
         <v>1377</v>
       </c>
-      <c r="B324" s="13" t="s">
+      <c r="C324" s="13" t="s">
         <v>1378</v>
       </c>
-      <c r="C324" s="13" t="s">
+      <c r="D324" s="13" t="s">
         <v>1379</v>
-      </c>
-      <c r="D324" s="13" t="s">
-        <v>1380</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="13" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B325" s="13" t="s">
         <v>1381</v>
       </c>
-      <c r="B325" s="13" t="s">
+      <c r="C325" s="13" t="s">
         <v>1382</v>
       </c>
-      <c r="C325" s="13" t="s">
+      <c r="D325" s="13" t="s">
         <v>1383</v>
-      </c>
-      <c r="D325" s="13" t="s">
-        <v>1384</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="13" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B326" s="13" t="s">
         <v>1385</v>
       </c>
-      <c r="B326" s="13" t="s">
+      <c r="C326" s="13" t="s">
         <v>1386</v>
       </c>
-      <c r="C326" s="13" t="s">
+      <c r="D326" s="13" t="s">
         <v>1387</v>
-      </c>
-      <c r="D326" s="13" t="s">
-        <v>1388</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="13" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B327" s="13" t="s">
         <v>1389</v>
       </c>
-      <c r="B327" s="13" t="s">
+      <c r="C327" s="13" t="s">
         <v>1390</v>
       </c>
-      <c r="C327" s="13" t="s">
+      <c r="D327" s="13" t="s">
         <v>1391</v>
-      </c>
-      <c r="D327" s="13" t="s">
-        <v>1392</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="13" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B328" s="13" t="s">
         <v>1393</v>
       </c>
-      <c r="B328" s="13" t="s">
+      <c r="C328" s="13" t="s">
         <v>1394</v>
       </c>
-      <c r="C328" s="13" t="s">
+      <c r="D328" s="13" t="s">
         <v>1395</v>
-      </c>
-      <c r="D328" s="13" t="s">
-        <v>1396</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="13" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B329" s="13" t="s">
         <v>1397</v>
       </c>
-      <c r="B329" s="13" t="s">
+      <c r="C329" s="13" t="s">
         <v>1398</v>
       </c>
-      <c r="C329" s="13" t="s">
+      <c r="D329" s="13" t="s">
         <v>1399</v>
-      </c>
-      <c r="D329" s="13" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="13" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B330" s="13" t="s">
         <v>1401</v>
       </c>
-      <c r="B330" s="13" t="s">
+      <c r="C330" s="13" t="s">
         <v>1402</v>
       </c>
-      <c r="C330" s="13" t="s">
+      <c r="D330" s="13" t="s">
         <v>1403</v>
-      </c>
-      <c r="D330" s="13" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="13" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B331" s="13" t="s">
         <v>1405</v>
       </c>
-      <c r="B331" s="13" t="s">
+      <c r="C331" s="13" t="s">
         <v>1406</v>
       </c>
-      <c r="C331" s="13" t="s">
+      <c r="D331" s="13" t="s">
         <v>1407</v>
-      </c>
-      <c r="D331" s="13" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="13" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B332" s="13" t="s">
         <v>1409</v>
       </c>
-      <c r="B332" s="13" t="s">
+      <c r="C332" s="13" t="s">
         <v>1410</v>
       </c>
-      <c r="C332" s="13" t="s">
+      <c r="D332" s="13" t="s">
         <v>1411</v>
-      </c>
-      <c r="D332" s="13" t="s">
-        <v>1412</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="13" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B333" s="13" t="s">
         <v>1413</v>
       </c>
-      <c r="B333" s="13" t="s">
+      <c r="C333" s="13" t="s">
         <v>1414</v>
       </c>
-      <c r="C333" s="13" t="s">
+      <c r="D333" s="13" t="s">
         <v>1415</v>
-      </c>
-      <c r="D333" s="13" t="s">
-        <v>1416</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="13" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B334" s="13" t="s">
         <v>1417</v>
       </c>
-      <c r="B334" s="13" t="s">
+      <c r="C334" s="13" t="s">
         <v>1418</v>
       </c>
-      <c r="C334" s="13" t="s">
+      <c r="D334" s="13" t="s">
         <v>1419</v>
-      </c>
-      <c r="D334" s="13" t="s">
-        <v>1420</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="13" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B335" s="13" t="s">
         <v>1421</v>
       </c>
-      <c r="B335" s="13" t="s">
+      <c r="C335" s="13" t="s">
         <v>1422</v>
       </c>
-      <c r="C335" s="13" t="s">
+      <c r="D335" s="13" t="s">
         <v>1423</v>
-      </c>
-      <c r="D335" s="13" t="s">
-        <v>1424</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="13" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B336" s="13" t="s">
         <v>1425</v>
       </c>
-      <c r="B336" s="13" t="s">
+      <c r="C336" s="13" t="s">
         <v>1426</v>
       </c>
-      <c r="C336" s="13" t="s">
+      <c r="D336" s="13" t="s">
         <v>1427</v>
-      </c>
-      <c r="D336" s="13" t="s">
-        <v>1428</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="13" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B337" s="13" t="s">
         <v>1429</v>
       </c>
-      <c r="B337" s="13" t="s">
+      <c r="C337" s="13" t="s">
         <v>1430</v>
       </c>
-      <c r="C337" s="13" t="s">
+      <c r="D337" s="13" t="s">
         <v>1431</v>
-      </c>
-      <c r="D337" s="13" t="s">
-        <v>1432</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="13" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B338" s="13" t="s">
         <v>1433</v>
       </c>
-      <c r="B338" s="13" t="s">
+      <c r="C338" s="13" t="s">
         <v>1434</v>
       </c>
-      <c r="C338" s="13" t="s">
+      <c r="D338" s="13" t="s">
         <v>1435</v>
       </c>
-      <c r="D338" s="13" t="s">
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="13" t="s">
         <v>1436</v>
       </c>
-    </row>
-    <row r="340" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="13" t="s">
+      <c r="B339" s="13" t="s">
         <v>1437</v>
       </c>
-      <c r="B340" s="13" t="s">
+      <c r="C339" s="13" t="s">
         <v>1438</v>
       </c>
-      <c r="C340" s="14" t="s">
+      <c r="D339" s="13" t="s">
         <v>1439</v>
-      </c>
-      <c r="D340" s="14" t="s">
-        <v>1440</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="13" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B341" s="13" t="s">
         <v>1441</v>
       </c>
-      <c r="B341" s="13" t="s">
+      <c r="C341" s="14" t="s">
         <v>1442</v>
       </c>
-      <c r="C341" s="14" t="s">
+      <c r="D341" s="14" t="s">
         <v>1443</v>
-      </c>
-      <c r="D341" s="14" t="s">
-        <v>1444</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="13" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B342" s="13" t="s">
         <v>1445</v>
       </c>
-      <c r="B342" s="13" t="s">
+      <c r="C342" s="14" t="s">
         <v>1446</v>
       </c>
-      <c r="C342" s="14" t="s">
+      <c r="D342" s="14" t="s">
         <v>1447</v>
       </c>
-      <c r="D342" s="14" t="s">
+    </row>
+    <row r="343" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="13" t="s">
         <v>1448</v>
       </c>
-    </row>
-    <row r="343" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="13" t="s">
+      <c r="B343" s="13" t="s">
         <v>1449</v>
       </c>
-      <c r="B343" s="13" t="s">
+      <c r="C343" s="14" t="s">
         <v>1450</v>
       </c>
-      <c r="C343" s="14" t="s">
+      <c r="D343" s="14" t="s">
         <v>1451</v>
-      </c>
-      <c r="D343" s="14" t="s">
-        <v>1452</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="13" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B344" s="13" t="s">
         <v>1453</v>
       </c>
-      <c r="B344" s="13" t="s">
+      <c r="C344" s="14" t="s">
         <v>1454</v>
       </c>
-      <c r="C344" s="14" t="s">
+      <c r="D344" s="14" t="s">
         <v>1455</v>
       </c>
-      <c r="D344" s="14" t="s">
+    </row>
+    <row r="345" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="13" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="345" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="13" t="s">
+      <c r="B345" s="13" t="s">
         <v>1457</v>
       </c>
-      <c r="B345" s="13" t="s">
+      <c r="C345" s="14" t="s">
         <v>1458</v>
       </c>
-      <c r="C345" s="14" t="s">
+      <c r="D345" s="14" t="s">
         <v>1459</v>
-      </c>
-      <c r="D345" s="14" t="s">
-        <v>1460</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="13" t="s">
+        <v>1460</v>
+      </c>
+      <c r="B346" s="13" t="s">
         <v>1461</v>
       </c>
-      <c r="B346" s="13" t="s">
+      <c r="C346" s="14" t="s">
         <v>1462</v>
       </c>
-      <c r="C346" s="14" t="s">
+      <c r="D346" s="14" t="s">
         <v>1463</v>
-      </c>
-      <c r="D346" s="14" t="s">
-        <v>1464</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="13" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B347" s="13" t="s">
         <v>1465</v>
       </c>
-      <c r="B347" s="13" t="s">
+      <c r="C347" s="14" t="s">
         <v>1466</v>
       </c>
-      <c r="C347" s="14" t="s">
+      <c r="D347" s="14" t="s">
         <v>1467</v>
       </c>
-      <c r="D347" s="14" t="s">
+    </row>
+    <row r="348" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="13" t="s">
         <v>1468</v>
       </c>
-    </row>
-    <row r="348" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="13" t="s">
+      <c r="B348" s="13" t="s">
         <v>1469</v>
       </c>
-      <c r="B348" s="13" t="s">
+      <c r="C348" s="14" t="s">
         <v>1470</v>
       </c>
-      <c r="C348" s="14" t="s">
+      <c r="D348" s="14" t="s">
         <v>1471</v>
       </c>
-      <c r="D348" s="14" t="s">
+    </row>
+    <row r="349" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="13" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="349" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A349" s="13" t="s">
+      <c r="B349" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="B349" s="16" t="s">
+      <c r="C349" s="14" t="s">
         <v>1474</v>
       </c>
-      <c r="C349" s="14" t="s">
+      <c r="D349" s="14" t="s">
         <v>1475</v>
       </c>
-      <c r="D349" s="14" t="s">
+    </row>
+    <row r="350" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A350" s="13" t="s">
         <v>1476</v>
       </c>
-    </row>
-    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="13" t="s">
+      <c r="B350" s="16" t="s">
         <v>1477</v>
       </c>
-      <c r="B350" s="13" t="s">
+      <c r="C350" s="14" t="s">
         <v>1478</v>
       </c>
-      <c r="C350" s="13" t="s">
+      <c r="D350" s="14" t="s">
         <v>1479</v>
-      </c>
-      <c r="D350" s="13" t="s">
-        <v>1480</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="13" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B351" s="13" t="s">
         <v>1481</v>
       </c>
-      <c r="B351" s="13" t="s">
+      <c r="C351" s="13" t="s">
         <v>1482</v>
       </c>
-      <c r="C351" s="13" t="s">
+      <c r="D351" s="13" t="s">
         <v>1483</v>
       </c>
-      <c r="D351" s="13" t="s">
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="13" t="s">
         <v>1484</v>
       </c>
-    </row>
-    <row r="352" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="13" t="s">
+      <c r="B352" s="13" t="s">
         <v>1485</v>
       </c>
-      <c r="B352" s="13" t="s">
+      <c r="C352" s="13" t="s">
         <v>1486</v>
       </c>
-      <c r="C352" s="14" t="s">
-        <v>1084</v>
-      </c>
-      <c r="D352" s="14" t="s">
-        <v>1085</v>
+      <c r="D352" s="13" t="s">
+        <v>1487</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="13" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="B353" s="13" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="C353" s="14" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D353" s="14" t="s">
         <v>1088</v>
-      </c>
-      <c r="D353" s="14" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="13" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="B354" s="13" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="C354" s="14" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D354" s="14" t="s">
         <v>1092</v>
       </c>
-      <c r="D354" s="14" t="s">
-        <v>1093</v>
+    </row>
+    <row r="355" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="13" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B355" s="13" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C355" s="14" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D355" s="14" t="s">
+        <v>1096</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D1 B250:D258 B262:D262 B265:D290 B350:B1048576 C69:D211 C224:D224 C248:D339 D355:D1048576 C350:D351 C226:D229 C353:C1048576 B1:B348 C218:D221 C238:D238 C1:D64 C245:C246">
+  <conditionalFormatting sqref="B1:D1 B251:D259 B263:D263 B266:D291 B351:B1048576 C69:D212 C225:D225 C249:D340 D356:D1048576 C351:D352 C227:D230 C354:C1048576 B1:B349 C219:D222 C239:D239 C1:D64 C246:C247">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>